<commit_message>
enable xls output and refine frontend
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_48_rpt_PF_FinanceRecoverySummary.xlsx
+++ b/backend/reports/xlsx/Tab_48_rpt_PF_FinanceRecoverySummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B1AF4C-5940-1D47-8B00-52E792AD3AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0555436E-EDA0-B547-8BB3-A73D629EDE42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11320" yWindow="-21100" windowWidth="25600" windowHeight="21100" tabRatio="150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -101,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -109,41 +109,33 @@
     </font>
     <font>
       <sz val="20"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="BCSans-Regular"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="BCSans-Regular"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="BCSans-Regular"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="BCSans-Regular"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="BCSans-Regular"/>
     </font>
     <font>
       <sz val="7.5"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="BCSans-Regular"/>
     </font>
   </fonts>
   <fills count="3">
@@ -218,36 +210,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -636,126 +628,126 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="350" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" style="3"/>
-    <col min="4" max="4" width="32.5" style="3" customWidth="1"/>
-    <col min="5" max="14" width="13.83203125" style="3" customWidth="1"/>
-    <col min="15" max="16384" width="12.1640625" style="3"/>
+    <col min="1" max="1" width="7.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="2"/>
+    <col min="4" max="4" width="32.5" style="2" customWidth="1"/>
+    <col min="5" max="14" width="13.83203125" style="2" customWidth="1"/>
+    <col min="15" max="16384" width="12.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="26.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:14" ht="26.5" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="2"/>
+      <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" s="6" customFormat="1" ht="56.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="7" t="s">
+    <row r="2" spans="1:14" s="7" customFormat="1" ht="56.5" customHeight="1">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="21.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:14" ht="21.5" customHeight="1">
+      <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="9"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="D4" s="11">
+    <row r="4" spans="1:14">
+      <c r="D4" s="13">
         <f>SUM(D3:D3)</f>
         <v>0</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="13">
         <f>SUM(E3:E3)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="13">
         <f>SUM(F3:F3)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="13">
         <f>SUM(G3:G3)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="13">
         <f>SUM(H3:H3)</f>
         <v>0</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="13">
         <f>SUM(I3:I3)</f>
         <v>0</v>
       </c>
-      <c r="J4" s="11">
+      <c r="J4" s="13">
         <f>SUM(J3:J3)</f>
         <v>0</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="13">
         <f>SUM(K3:K3)</f>
         <v>0</v>
       </c>
-      <c r="L4" s="11">
+      <c r="L4" s="13">
         <f>SUM(L3:L3)</f>
         <v>0</v>
       </c>
-      <c r="M4" s="11">
+      <c r="M4" s="13">
         <f>SUM(M3:M3)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:14">
       <c r="A6" s="14" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
update utilities and templates
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_48_rpt_PF_FinanceRecoverySummary.xlsx
+++ b/backend/reports/xlsx/Tab_48_rpt_PF_FinanceRecoverySummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0555436E-EDA0-B547-8BB3-A73D629EDE42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA8F0978-800F-DF4C-B21A-26B7D09FC9B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11320" yWindow="-21100" windowWidth="25600" windowHeight="21100" tabRatio="150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Portfolio</t>
   </si>
@@ -42,9 +42,6 @@
   </si>
   <si>
     <t>Project Name</t>
-  </si>
-  <si>
-    <t>Reoverable (Current Fiscal)</t>
   </si>
   <si>
     <t>6309 Consulting Fees</t>
@@ -88,20 +85,74 @@
     <t>FINANCE RECOVERY Project Summary FORECAST AS OF {$d} for Fiscal {d.fiscal}</t>
   </si>
   <si>
-    <t>{$r.portfolio_name}</t>
-  </si>
-  <si>
-    <t>{#d = d.date:formatD(YYYY-MM-DD)}{#r = d.report[i]} {#rp = d.report[i].projects[i]} {#rt = d.report[i].portfolio_totals} {#rp1 = d.report[i].projects[i+1]} {#r1= d.report[i+1]} {#gt = d.grand_totals}</t>
+    <t>{#r = d.report[i]}</t>
+  </si>
+  <si>
+    <t>{#r1= d.report[i+1]}</t>
+  </si>
+  <si>
+    <t>{#rp = d.report[i].projects[i]}</t>
+  </si>
+  <si>
+    <t>{#rp1 = d.report[i].projects[i+1]}</t>
+  </si>
+  <si>
+    <t>{#rt = d.report[i].portfolio_totals}</t>
+  </si>
+  <si>
+    <t>{#gt = d.grand_totals}</t>
+  </si>
+  <si>
+    <t>{$rp.project_name}</t>
+  </si>
+  <si>
+    <t>{$rp.project_number}</t>
+  </si>
+  <si>
+    <t>Total Recoveries For Projects (current FY)</t>
+  </si>
+  <si>
+    <t>{$rp.current_fy_total_recoverable}</t>
+  </si>
+  <si>
+    <t>{$rp.portfolio_name}</t>
+  </si>
+  <si>
+    <t>{$rp1.portfolio_name}</t>
+  </si>
+  <si>
+    <t>{$rp.consulting_fees}</t>
+  </si>
+  <si>
+    <t>{$rp.consulting_expenses}</t>
+  </si>
+  <si>
+    <t>{$rp.operational_contracts_fees}</t>
+  </si>
+  <si>
+    <t>{$rp.operational_contracts_expenses}</t>
+  </si>
+  <si>
+    <t>{$rp.i_expenses}</t>
+  </si>
+  <si>
+    <t>{$rp.salary_costs}</t>
+  </si>
+  <si>
+    <t>{$rp.operating_costs}</t>
+  </si>
+  <si>
+    <t>{$rp.project_related_business_expenses}</t>
+  </si>
+  <si>
+    <t>{$rp.other_stobs}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-  </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -135,7 +186,18 @@
     </font>
     <font>
       <sz val="7.5"/>
-      <name val="BCSans-Regular"/>
+      <color indexed="8"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="BC Sans"/>
     </font>
   </fonts>
   <fills count="3">
@@ -147,7 +209,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
+        <fgColor rgb="FFEDEDED"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -158,19 +220,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="8"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -189,23 +238,34 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFBFBFBF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
-      <right style="thin">
-        <color indexed="8"/>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -214,34 +274,47 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -316,6 +389,9 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00424242"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFEDEDED"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -625,29 +701,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="350" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="331" zoomScaleNormal="331" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="7.5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" style="2"/>
-    <col min="4" max="4" width="32.5" style="2" customWidth="1"/>
-    <col min="5" max="14" width="13.83203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="28.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" style="2" customWidth="1"/>
+    <col min="7" max="8" width="13.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.83203125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.83203125" style="2" customWidth="1"/>
     <col min="15" max="16384" width="12.1640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="26.5" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" s="7" customFormat="1" ht="56.5" customHeight="1">
+    <row r="2" spans="1:14" s="7" customFormat="1" ht="56.5" customHeight="1" thickBot="1">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -658,99 +742,126 @@
         <v>2</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="21.5" customHeight="1">
-      <c r="A3" s="8" t="s">
+    </row>
+    <row r="3" spans="1:14" s="9" customFormat="1" ht="42">
+      <c r="A3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="M3" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="9" customFormat="1">
+      <c r="A4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="13"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="D4" s="13">
-        <f>SUM(D3:D3)</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="13">
-        <f>SUM(E3:E3)</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="13">
-        <f>SUM(F3:F3)</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="13">
-        <f>SUM(G3:G3)</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="13">
-        <f>SUM(H3:H3)</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="13">
-        <f>SUM(I3:I3)</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="13">
-        <f>SUM(J3:J3)</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="13">
-        <f>SUM(K3:K3)</f>
-        <v>0</v>
-      </c>
-      <c r="L4" s="13">
-        <f>SUM(L3:L3)</f>
-        <v>0</v>
-      </c>
-      <c r="M4" s="13">
-        <f>SUM(M3:M3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="14" t="s">
-        <v>15</v>
-      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
fix pr change requests #2
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_48_rpt_PF_FinanceRecoverySummary.xlsx
+++ b/backend/reports/xlsx/Tab_48_rpt_PF_FinanceRecoverySummary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAE6DD7-DBDA-2A4C-8C58-CF02FF66577D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F48B8B-1E1F-C94B-B719-A4EC5D38077B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" tabRatio="150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Portfolio</t>
   </si>
@@ -146,6 +146,9 @@
   </si>
   <si>
     <t>{$rp.other_stobs}</t>
+  </si>
+  <si>
+    <t>{#d = d.date}</t>
   </si>
 </sst>
 </file>
@@ -280,7 +283,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -303,6 +306,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -775,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="331" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16"/>
@@ -800,21 +806,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="57" customHeight="1">
-      <c r="A1" s="17"/>
-      <c r="B1" s="18" t="s">
+      <c r="A1" s="18"/>
+      <c r="B1" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
       <c r="N1" s="2"/>
     </row>
     <row r="2" spans="1:14" s="6" customFormat="1" ht="56.5" customHeight="1" thickBot="1">
@@ -859,95 +865,112 @@
       </c>
     </row>
     <row r="3" spans="1:14" s="8" customFormat="1" ht="42">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="16" t="s">
+      <c r="K3" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="M3" s="17" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:14" s="8" customFormat="1">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="12"/>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="7" t="s">
-        <v>13</v>
-      </c>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="13"/>
+    </row>
+    <row r="5" spans="1:14" s="8" customFormat="1">
+      <c r="A5" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="13"/>
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:14">
       <c r="A9" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:14">
       <c r="A10" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="7"/>
+    <row r="12" spans="1:14">
+      <c r="A12" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
descw-1364 eliminate zero-byte xls templates
* updated styling on tab 48 report
* added half a dozen missing templates
* next commit i'll add the rest so our docx templates and xls templates
  match # of files and filenames.
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_48_rpt_PF_FinanceRecoverySummary.xlsx
+++ b/backend/reports/xlsx/Tab_48_rpt_PF_FinanceRecoverySummary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F48B8B-1E1F-C94B-B719-A4EC5D38077B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEA39D0-EE03-864B-9A20-78A30DDFB894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" tabRatio="150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11320" yWindow="-21100" windowWidth="25600" windowHeight="21100" tabRatio="150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rpt_PF_FinanceRecoverySummary" sheetId="1" r:id="rId1"/>
@@ -155,7 +155,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -201,6 +201,11 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="BC Sans"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="0"/>
+      <name val="BCSans-Regular"/>
     </font>
   </fonts>
   <fills count="4">
@@ -218,7 +223,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6DAF1"/>
+        <fgColor rgb="FF003365"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -307,19 +312,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -337,7 +342,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -414,6 +419,7 @@
       <rgbColor rgb="00424242"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FF003365"/>
       <color rgb="FFC6DAF1"/>
       <color rgb="FFEDEDED"/>
     </mruColors>
@@ -436,20 +442,20 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>26736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>2005</xdr:rowOff>
+      <xdr:colOff>2411614</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>707092</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
+        <xdr:cNvPr id="2" name="Graphic 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E08538A9-39CA-83ED-6E6E-0613BC80055D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE719E45-552C-EC4B-BC3B-F51037A6BEC8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -460,8 +466,8 @@
       <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -471,8 +477,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="800100" cy="723900"/>
+          <a:off x="0" y="26736"/>
+          <a:ext cx="2411614" cy="680356"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -784,12 +790,12 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="331" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A2" sqref="A1:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="28.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="23.1640625" style="1" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
descw-1365 refactor report model(s)
</commit_message>
<xml_diff>
--- a/backend/reports/xlsx/Tab_48_rpt_PF_FinanceRecoverySummary.xlsx
+++ b/backend/reports/xlsx/Tab_48_rpt_PF_FinanceRecoverySummary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robrien/work/gdx-agreements-tracker/backend/reports/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BEA39D0-EE03-864B-9A20-78A30DDFB894}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E4C4B5-5A12-5045-8D43-43B722E7580F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11320" yWindow="-21100" windowWidth="25600" windowHeight="21100" tabRatio="150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14280" yWindow="-21100" windowWidth="51200" windowHeight="21100" tabRatio="150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rpt_PF_FinanceRecoverySummary" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Portfolio</t>
   </si>
@@ -149,13 +149,82 @@
   </si>
   <si>
     <t>{#d = d.date}</t>
+  </si>
+  <si>
+    <t>{$r.portfolio_name}</t>
+  </si>
+  <si>
+    <t>{$r1.portfolio_name}</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>{$gt.totals_recoveries_sum}</t>
+  </si>
+  <si>
+    <t>{$gt.consulting_fees_sum}</t>
+  </si>
+  <si>
+    <t>{$gt.consulting_expenses_sum}</t>
+  </si>
+  <si>
+    <t>{$gt.operational_contracts_fees_sum}</t>
+  </si>
+  <si>
+    <t>{$gt.operational_contracts_expenses_sum}</t>
+  </si>
+  <si>
+    <t>{$gt.i_expenses_sum}</t>
+  </si>
+  <si>
+    <t>{$gt.salary_costs_sum}</t>
+  </si>
+  <si>
+    <t>{$gt.operating_costs_sum}</t>
+  </si>
+  <si>
+    <t>{$gt.project_related_business_expenses_sum}</t>
+  </si>
+  <si>
+    <t>{$gt.other_stobs_sum}</t>
+  </si>
+  <si>
+    <t>{$rt.current_fy_total_recoverable}</t>
+  </si>
+  <si>
+    <t>{$rt.consulting_fees}</t>
+  </si>
+  <si>
+    <t>{$rt.consulting_expenses}</t>
+  </si>
+  <si>
+    <t>{$rt.operational_contracts_fees}</t>
+  </si>
+  <si>
+    <t>{$rt.operational_contracts_expenses}</t>
+  </si>
+  <si>
+    <t>{$rt.i_expenses}</t>
+  </si>
+  <si>
+    <t>{$rt.salary_costs}</t>
+  </si>
+  <si>
+    <t>{$rt.operating_costs}</t>
+  </si>
+  <si>
+    <t>{$rt.project_related_business_expenses}</t>
+  </si>
+  <si>
+    <t>{$r.portfolio_name} Total:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -207,8 +276,38 @@
       <color theme="0"/>
       <name val="BCSans-Regular"/>
     </font>
+    <font>
+      <b/>
+      <sz val="7.5"/>
+      <color indexed="8"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="BC Sans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="BC Sans"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,8 +326,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -284,11 +389,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFBFBFBF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFBFBFBF"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -312,27 +445,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -344,6 +459,44 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="14" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="12" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -419,9 +572,10 @@
       <rgbColor rgb="00424242"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFD9D9D9"/>
+      <color rgb="FFEDEDED"/>
       <color rgb="FF003365"/>
       <color rgb="FFC6DAF1"/>
-      <color rgb="FFEDEDED"/>
     </mruColors>
   </colors>
   <extLst>
@@ -787,10 +941,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="331" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:M11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.1640625" defaultRowHeight="16"/>
@@ -812,24 +966,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="57" customHeight="1">
-      <c r="A1" s="18"/>
-      <c r="B1" s="19" t="s">
+      <c r="A1" s="12"/>
+      <c r="B1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:14" s="6" customFormat="1" ht="56.5" customHeight="1" thickBot="1">
+    <row r="2" spans="1:14" s="6" customFormat="1" ht="56.5" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -870,113 +1024,215 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="8" customFormat="1" ht="42">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:14" s="6" customFormat="1" ht="56.5" customHeight="1" thickBot="1">
+      <c r="A3" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="15"/>
+    </row>
+    <row r="4" spans="1:14" s="8" customFormat="1" ht="43" thickBot="1">
+      <c r="A4" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G4" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="J4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K4" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="M3" s="17" t="s">
+      <c r="M4" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="8" customFormat="1">
-      <c r="A4" s="10" t="s">
+    <row r="5" spans="1:14" s="8" customFormat="1" ht="17" thickBot="1">
+      <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="13"/>
-    </row>
-    <row r="5" spans="1:14" s="8" customFormat="1">
-      <c r="A5" s="9" t="s">
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="11"/>
+    </row>
+    <row r="6" spans="1:14" s="8" customFormat="1" ht="42">
+      <c r="A6" s="23"/>
+      <c r="B6" s="23"/>
+      <c r="C6" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6" s="21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="17" thickBot="1">
+      <c r="A7" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22"/>
+    </row>
+    <row r="8" spans="1:14" ht="33" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="K8" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="M8" s="25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" s="7"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" s="7"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" s="7"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="13"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="13"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="7" t="s">
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
-      <c r="A7" s="7" t="s">
+    <row r="14" spans="1:14">
+      <c r="A14" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
-      <c r="A8" s="7" t="s">
+    <row r="15" spans="1:14">
+      <c r="A15" s="7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
-      <c r="A9" s="7" t="s">
+    <row r="16" spans="1:14">
+      <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="7" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
-      <c r="A11" s="7" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>